<commit_message>
test-2 images and files
</commit_message>
<xml_diff>
--- a/output/invoice_page_1.jpg.txt.xlsx
+++ b/output/invoice_page_1.jpg.txt.xlsx
@@ -488,15 +488,15 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WSUGSTIR-</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>29AAFCA0924K1ZN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -506,13 +506,13 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.79</v>
+        <v>0.92</v>
       </c>
       <c r="I2" t="n">
-        <v>0.71</v>
+        <v>0.99</v>
       </c>
       <c r="J2" t="n">
-        <v>0.97</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>